<commit_message>
corrected KN99alpha to TDY451
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0648.xlsx
+++ b/bioSample/bioSample_0648.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21E8A8C-FA60-D442-AFC6-BEACBE72DD91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB2F82E-D18C-C841-A722-27A64C78757B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>90minuteInduction</t>
   </si>
   <si>
-    <t>KN99alpha</t>
-  </si>
-  <si>
     <t>CNAG_00000</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>CNAG_00440</t>
+  </si>
+  <si>
+    <t>TDY451</t>
   </si>
 </sst>
 </file>
@@ -477,12 +477,14 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1048576"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1023" width="8.83203125" customWidth="1"/>
+    <col min="1" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="1023" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -531,13 +533,13 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>90</v>
@@ -560,13 +562,13 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3">
         <v>90</v>
@@ -589,13 +591,13 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4">
         <v>90</v>
@@ -618,13 +620,13 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5">
         <v>90</v>
@@ -647,13 +649,13 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6">
         <v>90</v>
@@ -676,13 +678,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7">
         <v>90</v>
@@ -705,13 +707,13 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8">
         <v>90</v>
@@ -734,13 +736,13 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9">
         <v>90</v>
@@ -763,13 +765,13 @@
         <v>12</v>
       </c>
       <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10">
         <v>90</v>
@@ -780,7 +782,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -792,13 +794,13 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11">
         <v>90</v>
@@ -809,7 +811,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -821,13 +823,13 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12">
         <v>90</v>
@@ -838,22 +840,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13">
         <v>90</v>
@@ -864,7 +866,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -876,10 +878,10 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14">
         <v>90</v>
@@ -890,22 +892,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15">
         <v>90</v>
@@ -916,7 +918,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -928,13 +930,13 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
         <v>22</v>
       </c>
-      <c r="G16" t="s">
-        <v>23</v>
-      </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16">
         <v>90</v>
@@ -945,7 +947,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -957,13 +959,13 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
         <v>22</v>
       </c>
-      <c r="G17" t="s">
-        <v>23</v>
-      </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17">
         <v>90</v>
@@ -974,7 +976,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -986,13 +988,13 @@
         <v>12</v>
       </c>
       <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
         <v>22</v>
       </c>
-      <c r="G18" t="s">
-        <v>23</v>
-      </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I18">
         <v>90</v>

</xml_diff>